<commit_message>
Oprydning og færdiggørelse af forbedret OT opsamling
</commit_message>
<xml_diff>
--- a/P3/Results/Data/Gips/AllOTResults.xlsx
+++ b/P3/Results/Data/Gips/AllOTResults.xlsx
@@ -7,6 +7,12 @@
   </bookViews>
   <sheets>
     <sheet name="Gypsum6g" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Gypsum12g" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Gypsum18g" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Gypsum30g" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Gypsum45g" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Gypsum55g" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Gypsum65g" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -828,4 +834,1576 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="73" customWidth="1" min="1" max="1"/>
+    <col width="44" customWidth="1" min="2" max="2"/>
+    <col width="43" customWidth="1" min="3" max="3"/>
+    <col width="27" customWidth="1" min="4" max="4"/>
+    <col width="26" customWidth="1" min="5" max="5"/>
+    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="11" customWidth="1" min="7" max="7"/>
+    <col width="14" customWidth="1" min="8" max="8"/>
+    <col width="13" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Filename</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>PSNR Ground checker diff Reference checker</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>PSNR Ground checker diff Enhanced checker</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Reference</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Enhanced</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Dehazed</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>AG Ground</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>AG Reference</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>AG Enhanced</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>AG Dehazed</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Beside_Camera_light10_exp75731.0_20242011_144931.png</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>12.76</v>
+      </c>
+      <c r="C2" t="n">
+        <v>15.7</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-23.51</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-5.81</v>
+      </c>
+      <c r="F2" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="G2" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H2" t="n">
+        <v>4.14</v>
+      </c>
+      <c r="I2" t="n">
+        <v>16.98</v>
+      </c>
+      <c r="J2" t="n">
+        <v>6.91</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Beside_Camera_light5_exp112596.0_20242011_145005.png</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>12.14</v>
+      </c>
+      <c r="C3" t="n">
+        <v>15.42</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-17.41</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-4.24</v>
+      </c>
+      <c r="F3" t="n">
+        <v>16.8</v>
+      </c>
+      <c r="G3" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H3" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="I3" t="n">
+        <v>17.34</v>
+      </c>
+      <c r="J3" t="n">
+        <v>6.66</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Green_Beside_Camera_light10_exp241011.0_20242011_145643.png</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>15.16</v>
+      </c>
+      <c r="C4" t="n">
+        <v>15.19</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-40.94</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-2.37</v>
+      </c>
+      <c r="F4" t="n">
+        <v>10.87</v>
+      </c>
+      <c r="G4" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H4" t="n">
+        <v>7.34</v>
+      </c>
+      <c r="I4" t="n">
+        <v>17.88</v>
+      </c>
+      <c r="J4" t="n">
+        <v>9.869999999999999</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Green_Beside_Camera_light5_exp229371.0_20242011_145511.png</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>13.87</v>
+      </c>
+      <c r="C5" t="n">
+        <v>15.45</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-24.06</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-4.44</v>
+      </c>
+      <c r="F5" t="n">
+        <v>14.99</v>
+      </c>
+      <c r="G5" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H5" t="n">
+        <v>6.16</v>
+      </c>
+      <c r="I5" t="n">
+        <v>19.87</v>
+      </c>
+      <c r="J5" t="n">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Green_InFront_Camera_light10_exp79723.0_20242011_145354.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Green_InFront_Camera_light5_exp120641.0_20242011_145421.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Green_Right_Side_light10_exp179872.0_20242011_145732.png</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>15.06</v>
+      </c>
+      <c r="C8" t="n">
+        <v>14.89</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-36.03</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-1.51</v>
+      </c>
+      <c r="F8" t="n">
+        <v>11.06</v>
+      </c>
+      <c r="G8" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H8" t="n">
+        <v>7.33</v>
+      </c>
+      <c r="I8" t="n">
+        <v>19.2</v>
+      </c>
+      <c r="J8" t="n">
+        <v>10.06</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Green_Right_Side_light5_exp200093.0_20242011_145809.png</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>14.96</v>
+      </c>
+      <c r="C9" t="n">
+        <v>14.99</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-23.44</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-2.69</v>
+      </c>
+      <c r="F9" t="n">
+        <v>15.02</v>
+      </c>
+      <c r="G9" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H9" t="n">
+        <v>6.48</v>
+      </c>
+      <c r="I9" t="n">
+        <v>19.72</v>
+      </c>
+      <c r="J9" t="n">
+        <v>8.369999999999999</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>InFront_Camera_light10_exp39957.0_20242011_145308.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>InFront_Camera_light5_exp68580.0_20242011_145218.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Right_Side_light10_exp48796.0_20242011_145054.png</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>13.76</v>
+      </c>
+      <c r="C12" t="n">
+        <v>15.09</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-16.26</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-1.38</v>
+      </c>
+      <c r="F12" t="n">
+        <v>17.24</v>
+      </c>
+      <c r="G12" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H12" t="n">
+        <v>5.04</v>
+      </c>
+      <c r="I12" t="n">
+        <v>16.43</v>
+      </c>
+      <c r="J12" t="n">
+        <v>6.82</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Right_Side_light5_exp95117.0_20242011_145125.png</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>13.82</v>
+      </c>
+      <c r="C13" t="n">
+        <v>15.45</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-18.12</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-1.48</v>
+      </c>
+      <c r="F13" t="n">
+        <v>16.76</v>
+      </c>
+      <c r="G13" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H13" t="n">
+        <v>5.18</v>
+      </c>
+      <c r="I13" t="n">
+        <v>16.46</v>
+      </c>
+      <c r="J13" t="n">
+        <v>7.15</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Underwater_Beside_Camera_lightxUnderCam_exp231735.0_20242011_145948.png</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>13.78</v>
+      </c>
+      <c r="C14" t="n">
+        <v>14.92</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-18.29</v>
+      </c>
+      <c r="E14" t="n">
+        <v>10.51</v>
+      </c>
+      <c r="F14" t="n">
+        <v>11.57</v>
+      </c>
+      <c r="G14" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H14" t="n">
+        <v>7.36</v>
+      </c>
+      <c r="I14" t="n">
+        <v>9.65</v>
+      </c>
+      <c r="J14" t="n">
+        <v>8.970000000000001</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Underwater_Beside_Camera_lightx_exp248261.0_20242011_145857.png</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>16.25</v>
+      </c>
+      <c r="C15" t="n">
+        <v>15.11</v>
+      </c>
+      <c r="D15" t="n">
+        <v>-16.56</v>
+      </c>
+      <c r="E15" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="F15" t="n">
+        <v>14.15</v>
+      </c>
+      <c r="G15" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H15" t="n">
+        <v>6.82</v>
+      </c>
+      <c r="I15" t="n">
+        <v>11.55</v>
+      </c>
+      <c r="J15" t="n">
+        <v>8.19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="65" customWidth="1" min="1" max="1"/>
+    <col width="44" customWidth="1" min="2" max="2"/>
+    <col width="43" customWidth="1" min="3" max="3"/>
+    <col width="27" customWidth="1" min="4" max="4"/>
+    <col width="26" customWidth="1" min="5" max="5"/>
+    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="11" customWidth="1" min="7" max="7"/>
+    <col width="14" customWidth="1" min="8" max="8"/>
+    <col width="13" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Filename</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>PSNR Ground checker diff Reference checker</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>PSNR Ground checker diff Enhanced checker</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Reference</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Enhanced</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Dehazed</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>AG Ground</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>AG Reference</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>AG Enhanced</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>AG Dehazed</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Beside_Camera_light10_exp100281.0_20242011_151124.png</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>13.91</v>
+      </c>
+      <c r="C2" t="n">
+        <v>16.39</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-33.51</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-4.81</v>
+      </c>
+      <c r="F2" t="n">
+        <v>13.54</v>
+      </c>
+      <c r="G2" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H2" t="n">
+        <v>4.32</v>
+      </c>
+      <c r="I2" t="n">
+        <v>15.68</v>
+      </c>
+      <c r="J2" t="n">
+        <v>7.56</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Beside_Camera_light5_exp152620.0_20242011_151037.png</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>13.82</v>
+      </c>
+      <c r="C3" t="n">
+        <v>16.41</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-36.19</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-6.58</v>
+      </c>
+      <c r="F3" t="n">
+        <v>13.14</v>
+      </c>
+      <c r="G3" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H3" t="n">
+        <v>4.51</v>
+      </c>
+      <c r="I3" t="n">
+        <v>16.21</v>
+      </c>
+      <c r="J3" t="n">
+        <v>7.78</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Green_Beside_Camera_light10_exp189605.0_20242011_150407.png</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>13.97</v>
+      </c>
+      <c r="C4" t="n">
+        <v>16.47</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-42.35</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-8.76</v>
+      </c>
+      <c r="F4" t="n">
+        <v>12.1</v>
+      </c>
+      <c r="G4" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H4" t="n">
+        <v>4.79</v>
+      </c>
+      <c r="I4" t="n">
+        <v>20.62</v>
+      </c>
+      <c r="J4" t="n">
+        <v>8.19</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Green_Beside_Camera_light5_exp190102.0_20242011_150447.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Green_InFront_Camera_light10_exp93051.0_20242011_150612.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Green_InFront_Camera_light5_exp100182.0_20242011_150527.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Green_Right_Side_light10_exp127096.0_20242011_150322.png</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>14</v>
+      </c>
+      <c r="C8" t="n">
+        <v>16.28</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-43.59</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-11.26</v>
+      </c>
+      <c r="F8" t="n">
+        <v>12.96</v>
+      </c>
+      <c r="G8" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H8" t="n">
+        <v>5.08</v>
+      </c>
+      <c r="I8" t="n">
+        <v>23.97</v>
+      </c>
+      <c r="J8" t="n">
+        <v>7.72</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Green_Right_Side_light5_exp128189.0_20242011_150250.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>InFront_Camera_light10_exp63932.0_20242011_150912.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>InFront_Camera_light5_exp81670.0_20242011_150947.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Right_Side_light10_exp54596.0_20242011_151201.png</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>14.32</v>
+      </c>
+      <c r="C12" t="n">
+        <v>15.67</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-28.68</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-3.81</v>
+      </c>
+      <c r="F12" t="n">
+        <v>15.2</v>
+      </c>
+      <c r="G12" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H12" t="n">
+        <v>4.78</v>
+      </c>
+      <c r="I12" t="n">
+        <v>15.91</v>
+      </c>
+      <c r="J12" t="n">
+        <v>7.15</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Right_Side_light5_exp107631.0_20242011_151240.png</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>14.5</v>
+      </c>
+      <c r="C13" t="n">
+        <v>15.77</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-35.65</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-3.37</v>
+      </c>
+      <c r="F13" t="n">
+        <v>13.65</v>
+      </c>
+      <c r="G13" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H13" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="I13" t="n">
+        <v>15.29</v>
+      </c>
+      <c r="J13" t="n">
+        <v>7.91</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Underwater_Beside_Camera_lightx_exp278830.0_20242011_151328.png</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>14.78</v>
+      </c>
+      <c r="C14" t="n">
+        <v>15.85</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-20.84</v>
+      </c>
+      <c r="E14" t="n">
+        <v>3.38</v>
+      </c>
+      <c r="F14" t="n">
+        <v>16.46</v>
+      </c>
+      <c r="G14" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H14" t="n">
+        <v>5.08</v>
+      </c>
+      <c r="I14" t="n">
+        <v>12.81</v>
+      </c>
+      <c r="J14" t="n">
+        <v>6.41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="65" customWidth="1" min="1" max="1"/>
+    <col width="44" customWidth="1" min="2" max="2"/>
+    <col width="43" customWidth="1" min="3" max="3"/>
+    <col width="27" customWidth="1" min="4" max="4"/>
+    <col width="26" customWidth="1" min="5" max="5"/>
+    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="11" customWidth="1" min="7" max="7"/>
+    <col width="14" customWidth="1" min="8" max="8"/>
+    <col width="13" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Filename</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>PSNR Ground checker diff Reference checker</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>PSNR Ground checker diff Enhanced checker</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Reference</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Enhanced</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Dehazed</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>AG Ground</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>AG Reference</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>AG Enhanced</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>AG Dehazed</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Beside_Camera_light10_exp64568.0_20242011_152032.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Beside_Camera_light5_exp98057.0_20242011_151949.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Green_Beside_Camera_light10_exp161658.0_20242011_152545.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Green_Beside_Camera_light5_exp217592.0_20242011_152621.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Green_InFront_Camera_light10_exp67646.0_20242011_152410.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Green_InFront_Camera_light5_exp122150.0_20242011_152303.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Green_Right_Side_light10_exp122448.0_20242011_152721.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Green_Right_Side_light5_exp177548.0_20242011_152655.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>InFront_Camera_light10_exp27364.0_20242011_152119.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>InFront_Camera_light5_exp49889.0_20242011_152153.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Right_Side_light10_exp50604.0_20242011_151821.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Right_Side_light5_exp69553.0_20242011_151854.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Underwater_Beside_Camera_lightx_exp500005.0_20242011_152821.png</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>10.76</v>
+      </c>
+      <c r="C14" t="n">
+        <v>16.63</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-73.70999999999999</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-3.69</v>
+      </c>
+      <c r="F14" t="n">
+        <v>7.35</v>
+      </c>
+      <c r="G14" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H14" t="n">
+        <v>5.33</v>
+      </c>
+      <c r="I14" t="n">
+        <v>12.13</v>
+      </c>
+      <c r="J14" t="n">
+        <v>8.609999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="65" customWidth="1" min="1" max="1"/>
+    <col width="44" customWidth="1" min="2" max="2"/>
+    <col width="43" customWidth="1" min="3" max="3"/>
+    <col width="27" customWidth="1" min="4" max="4"/>
+    <col width="26" customWidth="1" min="5" max="5"/>
+    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="11" customWidth="1" min="7" max="7"/>
+    <col width="14" customWidth="1" min="8" max="8"/>
+    <col width="13" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Filename</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>PSNR Ground checker diff Reference checker</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>PSNR Ground checker diff Enhanced checker</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Reference</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Enhanced</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Dehazed</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>AG Ground</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>AG Reference</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>AG Enhanced</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>AG Dehazed</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Beside_Camera_light10_exp51875.0_20242011_153755.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Beside_Camera_light5_exp79008.0_20242011_153722.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Green_Beside_Camera_light10_exp95713.0_20242011_153324.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Green_Beside_Camera_light5_exp131804.0_20242011_153301.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Green_InFront_Camera_light10_exp65918.0_20242011_153356.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Green_InFront_Camera_light5_exp103439.0_20242011_153428.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Green_Right_Side_light10_exp74976.0_20242011_153139.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Green_Right_Side_light5_exp114245.0_20242011_153211.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>InFront_Camera_light10_exp25100.0_20242011_153617.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>InFront_Camera_light5_exp43989.0_20242011_153647.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Right_Side_light10_exp36283.0_20242011_153853.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Right_Side_light5_exp66355.0_20242011_153923.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Underwater_Beside_Camera_lightx_exp220750.0_20242011_153524.png</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="65" customWidth="1" min="1" max="1"/>
+    <col width="44" customWidth="1" min="2" max="2"/>
+    <col width="43" customWidth="1" min="3" max="3"/>
+    <col width="27" customWidth="1" min="4" max="4"/>
+    <col width="26" customWidth="1" min="5" max="5"/>
+    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="11" customWidth="1" min="7" max="7"/>
+    <col width="14" customWidth="1" min="8" max="8"/>
+    <col width="13" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Filename</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>PSNR Ground checker diff Reference checker</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>PSNR Ground checker diff Enhanced checker</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Reference</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Enhanced</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Dehazed</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>AG Ground</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>AG Reference</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>AG Enhanced</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>AG Dehazed</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Beside_Camera_light10_exp47227.0_20242011_154336.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Beside_Camera_light10_exp47227.0_20242011_154346.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Beside_Camera_light5_exp72394.0_20242011_154420.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Green_Beside_Camera_light10_exp97203.0_20242011_154748.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Green_Beside_Camera_light5_exp136591.0_20242011_154723.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Green_InFront_Camera_light10_exp60516.0_20242011_154617.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Green_InFront_Camera_light5_exp93349.0_20242011_154645.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Green_Right_Side_light10_exp84470.0_20242011_154823.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Green_Right_Side_light5_exp119211.0_20242011_154852.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>InFront_Camera_light10_exp22220.0_20242011_154529.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>InFront_Camera_light5_exp43116.0_20242011_154459.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Right_Side_light10_exp27444.0_20242011_154300.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Right_Side_light5_exp38130.0_20242011_154213.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Underwater_Beside_Camera_lightx_exp231159.0_20242011_154941.png</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="78" customWidth="1" min="1" max="1"/>
+    <col width="44" customWidth="1" min="2" max="2"/>
+    <col width="43" customWidth="1" min="3" max="3"/>
+    <col width="27" customWidth="1" min="4" max="4"/>
+    <col width="26" customWidth="1" min="5" max="5"/>
+    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="11" customWidth="1" min="7" max="7"/>
+    <col width="14" customWidth="1" min="8" max="8"/>
+    <col width="13" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Filename</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>PSNR Ground checker diff Reference checker</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>PSNR Ground checker diff Enhanced checker</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Reference</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Enhanced</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Dehazed</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>AG Ground</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>AG Reference</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>AG Enhanced</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>AG Dehazed</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Beside_Camera_light10_exp44943.0_20242011_161208.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Beside_Camera_light5_exp56523.0_20242011_161230.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Green_Beside_Camera_light10_exp114106.0_20242011_160940.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Green_Beside_Camera_light5_exp108544.0_20242011_160911.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Green_InFront_Camera_light10_exp59503.0_20242011_161006.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Green_InFront_Camera_light5_exp72870.0_20242011_161041.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Green_Right_Side_light10_exp76962.0_20242011_160800.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Green_Right_Side_light5_exp90131.0_20242011_160827.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>InFront_Camera_light10_exp20929.0_20242011_161137.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>InFront_Camera_light5_exp40911.0_20242011_161114.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Right_Side_light10_exp30503.0_20242011_161328.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Right_Side_light5_exp54954.0_20242011_161259.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Underwater_Beside_Camera_lightxCLOSE_exp500005.0_20242011_155535.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Underwater_Beside_Camera_lightxCLOSE_exp500005.0_20242011_155547.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Underwater_Beside_Camera_lightxCLOSE_exp500005.0_20242011_155609.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Underwater_Beside_Camera_lightxCLOSE_exp500005.0_20242011_155629.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Underwater_Right_of_Camera_Dark_room_light10_exp104770.0_20242011_160724.png</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>